<commit_message>
add sens slider option
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="9000" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
     <sheet name="Plan4" sheetId="4" r:id="rId4"/>
+    <sheet name="PLan5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>receitas</t>
   </si>
@@ -630,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -690,4 +691,79 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>